<commit_message>
opti log,optio page code example
</commit_message>
<xml_diff>
--- a/runner/Report.xlsx
+++ b/runner/Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>测试报告总概况</t>
   </si>
@@ -35,16 +35,16 @@
     <t>测试日期</t>
   </si>
   <si>
-    <t>'简书'</t>
-  </si>
-  <si>
-    <t>14M</t>
-  </si>
-  <si>
-    <t>17051515</t>
-  </si>
-  <si>
-    <t>2017-07-03 14:49:42</t>
+    <t>weblink</t>
+  </si>
+  <si>
+    <t>25M</t>
+  </si>
+  <si>
+    <t>1.2.3</t>
+  </si>
+  <si>
+    <t>2017-09-23 17:28:31</t>
   </si>
   <si>
     <t>用例总数</t>
@@ -59,7 +59,7 @@
     <t>测试耗时</t>
   </si>
   <si>
-    <t>27秒</t>
+    <t>120秒</t>
   </si>
   <si>
     <t>脚本语言</t>
@@ -80,28 +80,67 @@
     <t>用例介绍</t>
   </si>
   <si>
-    <t>用例名字</t>
+    <t>用例函数</t>
+  </si>
+  <si>
+    <t xml:space="preserve">操作步骤 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">检查点 </t>
   </si>
   <si>
     <t xml:space="preserve">测试结果 </t>
   </si>
   <si>
+    <t xml:space="preserve">备注 </t>
+  </si>
+  <si>
     <t>截图</t>
   </si>
   <si>
     <t>Huawei_H60-L02_android_4.4.2</t>
   </si>
   <si>
-    <t>test0003</t>
-  </si>
-  <si>
-    <t>发布文章</t>
-  </si>
-  <si>
-    <t>WriteTest</t>
+    <t>test0001</t>
+  </si>
+  <si>
+    <t>知识技术专区列表</t>
+  </si>
+  <si>
+    <t>TechZoneListTest</t>
+  </si>
+  <si>
+    <t>点击底部菜单的知识按钮;点击知识专区卡片;获取知识专区卡片列表的第一个数据项的标题值;获取知识专区列表卡片的第二个数据项的标题值;获取知识专区列表卡片的第三个数据项的标题值;点击左上角按钮回到列表页;</t>
+  </si>
+  <si>
+    <t>检查点步骤获取知识专区首页卡片列表的第一个数据项的标题值，并与详情页标题对比;获取知识专区首页卡片列表的第二个数据项的标题值，并与详情页标题对比;获取知识专区首页卡片列表的第三个数据项的标题值，并与详情页标题对比;</t>
+  </si>
+  <si>
+    <t>通过</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>test0002</t>
+  </si>
+  <si>
+    <t>知识技术专区详情页</t>
+  </si>
+  <si>
+    <t>TechZoneDetailTest</t>
+  </si>
+  <si>
+    <t>点击底部menu的知识;获取首页知识技术列表第一条数据，点击进入到详情页;</t>
+  </si>
+  <si>
+    <t>获取详情页到标题</t>
   </si>
   <si>
     <t>失败</t>
+  </si>
+  <si>
+    <t>请检查元素//*[@id="app"]/div/div[2]/section[2]/div[1]/div是否存在</t>
   </si>
 </sst>
 </file>
@@ -259,7 +298,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -334,20 +373,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="发布文章CheckPoint_1_NG.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="知识技术专区详情页CheckPoint_1_NG.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -360,7 +399,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3048000" y="571500"/>
+          <a:off x="4876800" y="952500"/>
           <a:ext cx="1028700" cy="1828800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -700,7 +739,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>15</v>
@@ -717,7 +756,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>16</v>
@@ -766,13 +805,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -782,8 +821,10 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1">
+    <row r="2" spans="1:9" ht="30" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -802,27 +843,72 @@
       <c r="F2" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="110" customHeight="1">
+    <row r="3" spans="1:9" ht="30" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="110" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>28</v>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
edit PageObject and yaml
</commit_message>
<xml_diff>
--- a/runner/Report.xlsx
+++ b/runner/Report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>测试报告总概况</t>
   </si>
@@ -44,7 +44,7 @@
     <t>1.2.3</t>
   </si>
   <si>
-    <t>2017-09-23 17:28:31</t>
+    <t>2017-10-18 14:39:30</t>
   </si>
   <si>
     <t>用例总数</t>
@@ -59,7 +59,7 @@
     <t>测试耗时</t>
   </si>
   <si>
-    <t>120秒</t>
+    <t>123秒</t>
   </si>
   <si>
     <t>脚本语言</t>
@@ -83,6 +83,9 @@
     <t>用例函数</t>
   </si>
   <si>
+    <t>前置条件</t>
+  </si>
+  <si>
     <t xml:space="preserve">操作步骤 </t>
   </si>
   <si>
@@ -98,10 +101,10 @@
     <t>截图</t>
   </si>
   <si>
-    <t>Huawei_H60-L02_android_4.4.2</t>
-  </si>
-  <si>
-    <t>test0001</t>
+    <t>HUAWEI_NEXT_android_6.0</t>
+  </si>
+  <si>
+    <t>test0003</t>
   </si>
   <si>
     <t>知识技术专区列表</t>
@@ -110,37 +113,52 @@
     <t>TechZoneListTest</t>
   </si>
   <si>
-    <t>点击底部菜单的知识按钮;点击知识专区卡片;获取知识专区卡片列表的第一个数据项的标题值;获取知识专区列表卡片的第二个数据项的标题值;获取知识专区列表卡片的第三个数据项的标题值;点击左上角按钮回到列表页;</t>
-  </si>
-  <si>
-    <t>检查点步骤获取知识专区首页卡片列表的第一个数据项的标题值，并与详情页标题对比;获取知识专区首页卡片列表的第二个数据项的标题值，并与详情页标题对比;获取知识专区首页卡片列表的第三个数据项的标题值，并与详情页标题对比;</t>
+    <t>技术卡片放在首页第一位</t>
+  </si>
+  <si>
+    <t>点击底部菜单的知识按钮;点击取消更新;点击技术专区卡片进入到技术专区列表;获取技术专区卡片列表的第一个数据项的标题值;获取技术专区列表卡片的第二个数据项的标题值;获取技术专区列表卡片的第三个数据项的标题值;点击左上角按钮回到列表页;</t>
+  </si>
+  <si>
+    <t>检查点步骤获取首页技术专区卡片列表的第一个数据项的标题值，并与详情页标题对比;获取首页技术专区卡片列表的第二个数据项的标题值，并与详情页标题对比;获取首页技术专区卡片列表的第三个数据项的标题值，并与详情页标题对比;</t>
+  </si>
+  <si>
+    <t>失败</t>
+  </si>
+  <si>
+    <t>首页到知识专区到列表三条数据和详情页到三条数据对不上。详情页三条数据为：['Linux下模拟网络损伤', 'A标签跳转前做校验', 'Linux下模拟网络损伤']。首页当前匹配数据为:由于参数配置错误导致安装部署失败问题案例及解决办法</t>
+  </si>
+  <si>
+    <t>test0002</t>
+  </si>
+  <si>
+    <t>知识技术专区详情页</t>
+  </si>
+  <si>
+    <t>TechZoneDetailTest</t>
+  </si>
+  <si>
+    <t>点击底部menu的知识;点击取消更新;获取首页知识技术列表第一条数据;点击首页技术列表第一条数据进入到详情页;</t>
+  </si>
+  <si>
+    <t>获取详情页到标题，并与首页第一条数据标题进行对比</t>
   </si>
   <si>
     <t>通过</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>test0002</t>
-  </si>
-  <si>
-    <t>知识技术专区详情页</t>
-  </si>
-  <si>
-    <t>TechZoneDetailTest</t>
-  </si>
-  <si>
-    <t>点击底部menu的知识;获取首页知识技术列表第一条数据，点击进入到详情页;</t>
-  </si>
-  <si>
-    <t>获取详情页到标题</t>
-  </si>
-  <si>
-    <t>失败</t>
-  </si>
-  <si>
-    <t>请检查元素//*[@id="app"]/div/div[2]/section[2]/div[1]/div是否存在</t>
+    <t>test0004</t>
+  </si>
+  <si>
+    <t>技术专区刷新</t>
+  </si>
+  <si>
+    <t>TechZoneRefreTest</t>
+  </si>
+  <si>
+    <t>点击底部菜单的知识按钮;点击取消更新;点击技术专区到刷新按钮;获取首页技术专区卡片列表的第一个数据项的标题值;获取首页技术专区卡片列表的第二个数据项的标题值;获取首页技术专区卡片列表的第三个数据项的标题值;点击技术专区卡片进入到技术专区列表;</t>
+  </si>
+  <si>
+    <t>检查点步骤获取技术专区卡片列表的第一个数据项的标题值;获取技术专区列表卡片的第二个数据项的标题值;获取技术专区列表卡片的第三个数据项的标题值;</t>
   </si>
 </sst>
 </file>
@@ -260,7 +278,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>接口测试统计</a:t>
+              <a:t>测试统计</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -298,7 +316,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
@@ -373,20 +391,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="知识技术专区详情页CheckPoint_1_NG.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="知识技术专区列表CheckPoint_1_NG.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -399,7 +417,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4876800" y="952500"/>
+          <a:off x="13096875" y="571500"/>
           <a:ext cx="1028700" cy="1828800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -739,7 +757,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>15</v>
@@ -756,7 +774,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>16</v>
@@ -805,13 +823,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
@@ -823,8 +853,9 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1">
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" ht="30" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
@@ -852,63 +883,104 @@
       <c r="I2" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" customHeight="1">
+      <c r="J2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="110" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1">
+      <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" ht="110" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
+        <v>42</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="30" customHeight="1">
+      <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="30" customHeight="1"/>
+    <row r="7" spans="1:10" ht="30" customHeight="1"/>
+    <row r="8" spans="1:10" ht="30" customHeight="1"/>
+    <row r="9" spans="1:10" ht="30" customHeight="1"/>
+    <row r="10" spans="1:10" ht="30" customHeight="1"/>
+    <row r="11" spans="1:10" ht="30" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>